<commit_message>
criando casos por regioes
</commit_message>
<xml_diff>
--- a/casos_por_estado.xlsx
+++ b/casos_por_estado.xlsx
@@ -460,10 +460,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2375</v>
+        <v>59</v>
       </c>
       <c r="D2" t="n">
-        <v>40.91</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="3">
@@ -476,10 +476,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1416</v>
+        <v>89</v>
       </c>
       <c r="D3" t="n">
-        <v>24.39</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>299</v>
+        <v>60</v>
       </c>
       <c r="D4" t="n">
-        <v>5.15</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="5">
@@ -508,10 +508,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>522</v>
+        <v>47</v>
       </c>
       <c r="D5" t="n">
-        <v>8.99</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -524,10 +524,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>519</v>
+        <v>253</v>
       </c>
       <c r="D6" t="n">
-        <v>8.94</v>
+        <v>4.36</v>
       </c>
     </row>
     <row r="7">
@@ -540,10 +540,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>762</v>
+        <v>168</v>
       </c>
       <c r="D7" t="n">
-        <v>13.13</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="8">
@@ -556,10 +556,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1381</v>
+        <v>1118</v>
       </c>
       <c r="D8" t="n">
-        <v>23.79</v>
+        <v>19.26</v>
       </c>
     </row>
     <row r="9">
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>452</v>
+        <v>170</v>
       </c>
       <c r="D9" t="n">
-        <v>7.79</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="10">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>854</v>
+        <v>270</v>
       </c>
       <c r="D10" t="n">
-        <v>14.71</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="11">

</xml_diff>